<commit_message>
Test connexion, pas résussi
</commit_message>
<xml_diff>
--- a/Info/Journal-de-Travail_ChasiDario.xlsx
+++ b/Info/Journal-de-Travail_ChasiDario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJETS\P_Mobile\ReadMe\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC41B221-A70E-4907-B781-4E5011DFB8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CF0C6A-AF8B-4907-8BB5-BC6510B1C7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -145,7 +145,16 @@
     <t>Recherche du fonctionnement de MAUI</t>
   </si>
   <si>
-    <t>Création des différents pages</t>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Création du sqlite</t>
+  </si>
+  <si>
+    <t>Mélange des projet, manque connexion api</t>
+  </si>
+  <si>
+    <t>Finalisation des différents pages de l'app</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1085,7 @@
                   <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.1875</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1094,7 +1103,7 @@
                   <c:v>5.2083333333333336E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2007,7 +2016,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2060,7 +2069,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 4 heurs 30 minutes</v>
+        <v>0 jours 11 heurs 15 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2075,15 +2084,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>480</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>150</v>
+        <v>195</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>270</v>
+        <v>675</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2258,15 +2267,19 @@
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B12" s="46">
-        <v>45380</v>
-      </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
+        <v>45404</v>
+      </c>
+      <c r="C12" s="47">
+        <v>2</v>
+      </c>
+      <c r="D12" s="48">
+        <v>15</v>
+      </c>
       <c r="E12" s="49" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F12" s="36" t="s">
         <v>34</v>
@@ -2283,15 +2296,25 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="str">
+      <c r="A13" s="16">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="36"/>
+        <v>18</v>
+      </c>
+      <c r="B13" s="50">
+        <v>45411</v>
+      </c>
+      <c r="C13" s="51">
+        <v>2</v>
+      </c>
+      <c r="D13" s="52">
+        <v>15</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>37</v>
+      </c>
       <c r="G13" s="56"/>
       <c r="M13" t="s">
         <v>8</v>
@@ -2304,16 +2327,28 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="str">
+      <c r="A14" s="8">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="55"/>
+        <v>19</v>
+      </c>
+      <c r="B14" s="46">
+        <v>45418</v>
+      </c>
+      <c r="C14" s="47">
+        <v>2</v>
+      </c>
+      <c r="D14" s="48">
+        <v>15</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="55" t="s">
+        <v>36</v>
+      </c>
       <c r="M14" t="s">
         <v>21</v>
       </c>
@@ -8664,11 +8699,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8676,7 +8711,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8768,7 +8803,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C11" s="39" t="str">
         <f>'Journal de travail'!M15</f>
@@ -8776,7 +8811,7 @@
       </c>
       <c r="D11" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -8785,7 +8820,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.10416666666666666</v>
+        <v>0.30208333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9022,15 +9057,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9039,6 +9065,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9061,14 +9096,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9077,4 +9104,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>